<commit_message>
checking pipeline run for commits
</commit_message>
<xml_diff>
--- a/heartbeat_base_input_template.xlsx
+++ b/heartbeat_base_input_template.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://docs.philips.com/personal/ananyak_s_philips_com/Documents/Saved Pictures/VS Files/heartbeat generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_496D3B2F467328FEE77960B543245E3FB48F8EF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{018BDD8A-CF34-4643-8A91-29EFC0819276}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_496D2167864BB4FEE77960B543245E3FB48F8EF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF603873-EDE7-4000-B741-12DC049132E3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>type</t>
   </si>
@@ -156,22 +155,13 @@
   </si>
   <si>
     <t>site</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tcp </t>
-  </si>
-  <si>
-    <t>udp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,14 +173,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,12 +210,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,119 +679,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3">
-        <v>25.1</v>
-      </c>
-      <c r="K3">
-        <v>55.16</v>
-      </c>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>44</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{FDDD5B17-4F99-4E1B-8639-F34732933163}">
-      <formula1>$A$2:$A$4</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BAA1F2C-391C-4028-B62B-394DD7706B10}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>